<commit_message>
removed redundant thousands label
</commit_message>
<xml_diff>
--- a/project/3point2barchart.xlsx
+++ b/project/3point2barchart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://testingcircle-my.sharepoint.com/personal/khanson_spartaglobal_com/Documents/Sparta/Training/SQL/Practical Exercise/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://testingcircle-my.sharepoint.com/personal/khanson_spartaglobal_com/Documents/Sparta/Training/SQL/Practical Exercise/SQLProject/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="11_B4E765BA8ADF1A091061005C784339F0E18053A4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5EB846CD-7A8F-E94D-A5D0-26C446D3B891}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="11_B4E765BA8ADF1A091061005C784339F0E18053A4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AEB2E2B4-AF17-F447-90F5-53FCDD66EA2C}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -269,79 +269,79 @@
                   <c:v>Aux joyeux ecclésiastiques</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Bigfoot Breweries</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Cooperativa de Quesos 'Las Cabras'</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Exotic Liquids</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Forêts d'érables</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Formaggi Fortini s.r.l.</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>G'day, Mate</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Gai pâturage</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Grandma Kelly's Homestead</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Heli Süßwaren GmbH &amp; Co. KG</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Karkki Oy</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Leka Trading</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Lyngbysild</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Ma Maison</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Mayumi's</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>New England Seafood Cannery</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>New Orleans Cajun Delights</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Nord-Ost-Fisch Handelsgesellschaft mbH</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Norske Meierier</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Pasta Buttini s.r.l.</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Pavlova, Ltd.</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>PB Knäckebröd AB</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>Plutzer Lebensmittelgroßmärkte AG</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Gai pâturage</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Pavlova, Ltd.</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>G'day, Mate</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Forêts d'érables</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Pasta Buttini s.r.l.</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Formaggi Fortini s.r.l.</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="23">
                   <c:v>Specialty Biscuits, Ltd.</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>Norske Meierier</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Leka Trading</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Grandma Kelly's Homestead</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Heli Süßwaren GmbH &amp; Co. KG</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Exotic Liquids</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>New Orleans Cajun Delights</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="24">
+                  <c:v>Svensk Sjöföda AB</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>Tokyo Traders</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Karkki Oy</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>New England Seafood Cannery</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Cooperativa de Quesos 'Las Cabras'</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Bigfoot Breweries</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Ma Maison</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Svensk Sjöföda AB</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Mayumi's</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>Nord-Ost-Fisch Handelsgesellschaft mbH</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>PB Knäckebröd AB</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Lyngbysild</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -356,79 +356,79 @@
                   <c:v>153691.28</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>22391.200000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25159.43</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32188.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>61587.57</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48225.163999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65626.77</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>117981.18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41953.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38653.417999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28442.728999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42017.644999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10221.174999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22154.636999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14736.754999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>26590.974999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>31167.99</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13424.197</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43141.51</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>50254.61</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>106459.77</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11724.06</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>145372.4</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>117981.18</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>106459.77</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>65626.77</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>61587.57</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>50254.61</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>48225.163999999997</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="23">
                   <c:v>46243.98</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>43141.51</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>42017.644999999997</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41953.3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>38653.417999999998</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>32188.06</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>31167.99</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="24">
+                  <c:v>20144.060000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>30526.34</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>28442.728999999999</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>26590.974999999999</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>25159.43</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>22391.200000000001</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>22154.636999999999</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>20144.060000000001</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>14736.754999999999</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>13424.197</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>11724.06</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>10221.174999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1318,7 +1318,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B89D916-62CC-9E4A-89AB-9074D95D3F98}" name="Table1" displayName="Table1" ref="A1:B27" totalsRowShown="0">
   <autoFilter ref="A1:B27" xr:uid="{D2D23239-2590-E847-AC4F-57E3775FD8C4}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B27">
-    <sortCondition descending="1" ref="B1:B27"/>
+    <sortCondition ref="A1:A27"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{0929214B-3D56-9641-B1EA-8255BBECE7BA}" name="Company Name"/>
@@ -1627,8 +1627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E9" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1654,202 +1654,202 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>145372.4</v>
+        <v>22391.200000000001</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>117981.18</v>
+        <v>25159.43</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>106459.77</v>
+        <v>32188.06</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>65626.77</v>
+        <v>61587.57</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>61587.57</v>
+        <v>48225.163999999997</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>50254.61</v>
+        <v>65626.77</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>48225.163999999997</v>
+        <v>117981.18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>46243.98</v>
+        <v>41953.3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>43141.51</v>
+        <v>38653.417999999998</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>42017.644999999997</v>
+        <v>28442.728999999999</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>41953.3</v>
+        <v>42017.644999999997</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>38653.417999999998</v>
+        <v>10221.174999999999</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>32188.06</v>
+        <v>22154.636999999999</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16">
-        <v>31167.99</v>
+        <v>14736.754999999999</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B17">
-        <v>30526.34</v>
+        <v>26590.974999999999</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B18">
-        <v>28442.728999999999</v>
+        <v>31167.99</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B19">
-        <v>26590.974999999999</v>
+        <v>13424.197</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B20">
-        <v>25159.43</v>
+        <v>43141.51</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B21">
-        <v>22391.200000000001</v>
+        <v>50254.61</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B22">
-        <v>22154.636999999999</v>
+        <v>106459.77</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B23">
-        <v>20144.060000000001</v>
+        <v>11724.06</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B24">
-        <v>14736.754999999999</v>
+        <v>145372.4</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B25">
-        <v>13424.197</v>
+        <v>46243.98</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B26">
-        <v>11724.06</v>
+        <v>20144.060000000001</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B27">
-        <v>10221.174999999999</v>
+        <v>30526.34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed target blank links
</commit_message>
<xml_diff>
--- a/project/3point2barchart.xlsx
+++ b/project/3point2barchart.xlsx
@@ -1627,8 +1627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>